<commit_message>
Found internal temp conversion in Conversion.xlsx, added math.asm, and began implenting conversion for internal temp sensor. Stuck right now needing a 16 bit subtraction.
</commit_message>
<xml_diff>
--- a/EELE465_Lab03/Doc/Conversion.xlsx
+++ b/EELE465_Lab03/Doc/Conversion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LM 19" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>T_actual</t>
   </si>
@@ -37,12 +37,15 @@
   <si>
     <t>Offset</t>
   </si>
+  <si>
+    <t>Error C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,6 +54,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -79,13 +90,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2458,11 +2470,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63809408"/>
-        <c:axId val="63835520"/>
+        <c:axId val="85116800"/>
+        <c:axId val="85400960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63809408"/>
+        <c:axId val="85116800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="350"/>
@@ -2470,12 +2482,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63835520"/>
+        <c:crossAx val="85400960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63835520"/>
+        <c:axId val="85400960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2483,7 +2495,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63809408"/>
+        <c:crossAx val="85116800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2496,7 +2508,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3711,23 +3723,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77585024"/>
-        <c:axId val="78070144"/>
+        <c:axId val="86833792"/>
+        <c:axId val="87318912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77585024"/>
+        <c:axId val="86833792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78070144"/>
+        <c:crossAx val="87318912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78070144"/>
+        <c:axId val="87318912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3735,7 +3747,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77585024"/>
+        <c:crossAx val="86833792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3748,7 +3760,564 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Internal!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T_actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Internal!$A$2:$A$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Internal!$B$2:$B$46</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>0.75353741229956483</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7133226198407883</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6731078273820117</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6328930349233062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5926782424645296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.552463450005822</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.512248657547048</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.472033865088273</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.431819072629565</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.391604280170856</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.351389487712147</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.311174695253374</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.270959902794598</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26.145170407921356</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.968690165757906</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.792209923594516</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.615729681431066</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.439249439267613</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>35.262769197104227</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37.086288954940777</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>38.909808712777391</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>40.733328470613941</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42.556848228450491</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44.380367986287098</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>46.203887744123648</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>48.027407501960262</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>49.850927259796812</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>51.674447017633362</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>53.497966775469976</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>55.321486533306526</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>57.145006291143133</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>58.968526048979683</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>60.792045806816233</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>62.615565564652847</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>64.439085322489404</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>66.262605080326011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Internal!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T_Aprox</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Internal!$A$2:$A$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>231</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Internal!$C$2:$C$46</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="45"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="61441152"/>
+        <c:axId val="60873728"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="61441152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="60873728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="60873728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61441152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3811,6 +4380,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4106,11 +4710,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C155" sqref="C155"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6684,7 +7288,7 @@
         <v>13</v>
       </c>
       <c r="D150" s="5">
-        <f t="shared" si="8"/>
+        <f>ROUND(B150-C150, 0)</f>
         <v>-2</v>
       </c>
     </row>
@@ -7411,32 +8015,650 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14" style="1" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="4"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>205</v>
+      </c>
+      <c r="B2" s="1">
+        <f>IF((3.3*A2/1023)&gt;0.7012,25-(0.7012-(3.3*A2/1023))/0.001769,25-(0.7012-(3.3*A2/1023))/0.001646)</f>
+        <v>0.75353741229956483</v>
+      </c>
+      <c r="C2" s="4">
+        <f>FLOOR((19*A2)/10,1) -388</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ROUND(B2-C2, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>206</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B43" si="0">IF((3.3*A3/1023)&gt;0.7012,25-(0.7012-(3.3*A3/1023))/0.001769,25-(0.7012-(3.3*A3/1023))/0.001646)</f>
+        <v>2.7133226198407883</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C37" si="1">FLOOR((19*A3)/10,1) -388</f>
         <v>3</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D37" si="2">ROUND(B3-C3, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>207</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6731078273820117</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>208</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6328930349233062</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>209</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>8.5926782424645296</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>210</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>10.552463450005822</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>211</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>12.512248657547048</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>212</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>14.472033865088273</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>213</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>16.431819072629565</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>214</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>18.391604280170856</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>215</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>20.351389487712147</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>216</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>22.311174695253374</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6">
+        <v>217</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>24.270959902794598</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6">
+        <v>218</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>26.145170407921356</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>219</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>27.968690165757906</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>220</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>29.792209923594516</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>221</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>31.615729681431066</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>222</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>33.439249439267613</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>223</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>35.262769197104227</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>224</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>37.086288954940777</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>225</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>38.909808712777391</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>226</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>40.733328470613941</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>227</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>42.556848228450491</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="D24" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>228</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>44.380367986287098</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D25" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>229</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>46.203887744123648</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D26" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>230</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>48.027407501960262</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D27" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>231</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>49.850927259796812</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>232</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>51.674447017633362</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="D29" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>233</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>53.497966775469976</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>234</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>55.321486533306526</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="D31" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>235</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>57.145006291143133</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>236</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>58.968526048979683</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>237</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>60.792045806816233</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>238</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>62.615565564652847</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>239</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>64.439085322489404</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>240</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>66.262605080326011</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="2"/>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Now converts w/o math_div_16, need to fix conversion formula
</commit_message>
<xml_diff>
--- a/EELE465_Lab03/Doc/Conversion.xlsx
+++ b/EELE465_Lab03/Doc/Conversion.xlsx
@@ -2470,11 +2470,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="85116800"/>
-        <c:axId val="85400960"/>
+        <c:axId val="62572416"/>
+        <c:axId val="62594432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85116800"/>
+        <c:axId val="62572416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="350"/>
@@ -2482,12 +2482,12 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85400960"/>
+        <c:crossAx val="62594432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85400960"/>
+        <c:axId val="62594432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,20 +2495,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85116800"/>
+        <c:crossAx val="62572416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2539,7 +2538,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3723,23 +3721,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86833792"/>
-        <c:axId val="87318912"/>
+        <c:axId val="65931904"/>
+        <c:axId val="65958272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86833792"/>
+        <c:axId val="65931904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87318912"/>
+        <c:crossAx val="65958272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87318912"/>
+        <c:axId val="65958272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3747,20 +3745,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86833792"/>
+        <c:crossAx val="65931904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4168,22 +4165,22 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>12</c:v>
@@ -4216,87 +4213,87 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>37</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>45</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>47</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>49</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>50</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>52</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>54</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>56</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>58</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>60</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>62</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>64</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>66</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>68</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="61441152"/>
-        <c:axId val="60873728"/>
+        <c:axId val="66104320"/>
+        <c:axId val="66114304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61441152"/>
+        <c:axId val="66104320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60873728"/>
+        <c:crossAx val="66114304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60873728"/>
+        <c:axId val="66114304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4304,7 +4301,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61441152"/>
+        <c:crossAx val="66104320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4317,7 +4314,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8053,12 +8050,12 @@
         <v>0.75353741229956483</v>
       </c>
       <c r="C2" s="4">
-        <f>FLOOR((19*A2)/10,1) -388</f>
-        <v>1</v>
+        <f>2*A2 -410</f>
+        <v>0</v>
       </c>
       <c r="D2" s="4">
         <f>ROUND(B2-C2, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8066,16 +8063,16 @@
         <v>206</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B43" si="0">IF((3.3*A3/1023)&gt;0.7012,25-(0.7012-(3.3*A3/1023))/0.001769,25-(0.7012-(3.3*A3/1023))/0.001646)</f>
+        <f t="shared" ref="B3:B37" si="0">IF((3.3*A3/1023)&gt;0.7012,25-(0.7012-(3.3*A3/1023))/0.001769,25-(0.7012-(3.3*A3/1023))/0.001646)</f>
         <v>2.7133226198407883</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C37" si="1">FLOOR((19*A3)/10,1) -388</f>
-        <v>3</v>
+        <f t="shared" ref="C3:C37" si="1">2*A3 -410</f>
+        <v>2</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D37" si="2">ROUND(B3-C3, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8088,11 +8085,11 @@
       </c>
       <c r="C4" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8105,11 +8102,11 @@
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8122,11 +8119,11 @@
       </c>
       <c r="C6" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -8139,11 +8136,11 @@
       </c>
       <c r="C7" s="4">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -8326,11 +8323,11 @@
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -8343,11 +8340,11 @@
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -8360,11 +8357,11 @@
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -8377,11 +8374,11 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -8394,11 +8391,11 @@
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -8411,11 +8408,11 @@
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -8428,11 +8425,11 @@
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -8445,11 +8442,11 @@
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -8462,11 +8459,11 @@
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -8479,11 +8476,11 @@
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -8496,11 +8493,11 @@
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -8513,11 +8510,11 @@
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -8530,11 +8527,11 @@
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -8547,11 +8544,11 @@
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -8564,11 +8561,11 @@
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -8581,11 +8578,11 @@
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -8598,11 +8595,11 @@
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -8615,11 +8612,11 @@
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -8632,11 +8629,11 @@
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -8649,11 +8646,11 @@
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed internal temp conversion
</commit_message>
<xml_diff>
--- a/EELE465_Lab03/Doc/Conversion.xlsx
+++ b/EELE465_Lab03/Doc/Conversion.xlsx
@@ -3912,112 +3912,112 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
-                  <c:v>0.75353741229956483</c:v>
+                  <c:v>49.246462587700435</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7133226198407883</c:v>
+                  <c:v>47.286677380159212</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6731078273820117</c:v>
+                  <c:v>45.326892172617988</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6328930349233062</c:v>
+                  <c:v>43.367106965076694</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.5926782424645296</c:v>
+                  <c:v>41.40732175753547</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.552463450005822</c:v>
+                  <c:v>39.447536549994176</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.512248657547048</c:v>
+                  <c:v>37.487751342452952</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.472033865088273</c:v>
+                  <c:v>35.527966134911729</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.431819072629565</c:v>
+                  <c:v>33.568180927370435</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.391604280170856</c:v>
+                  <c:v>31.608395719829144</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.351389487712147</c:v>
+                  <c:v>29.648610512287853</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.311174695253374</c:v>
+                  <c:v>27.688825304746626</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.270959902794598</c:v>
+                  <c:v>25.729040097205402</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.145170407921356</c:v>
+                  <c:v>23.854829592078644</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.968690165757906</c:v>
+                  <c:v>22.031309834242094</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.792209923594516</c:v>
+                  <c:v>20.207790076405484</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>31.615729681431066</c:v>
+                  <c:v>18.384270318568934</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33.439249439267613</c:v>
+                  <c:v>16.560750560732384</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35.262769197104227</c:v>
+                  <c:v>14.737230802895771</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>37.086288954940777</c:v>
+                  <c:v>12.913711045059223</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>38.909808712777391</c:v>
+                  <c:v>11.090191287222611</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>40.733328470613941</c:v>
+                  <c:v>9.2666715293860609</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42.556848228450491</c:v>
+                  <c:v>7.4431517715495126</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>44.380367986287098</c:v>
+                  <c:v>5.6196320137128986</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>46.203887744123648</c:v>
+                  <c:v>3.7961122558763485</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>48.027407501960262</c:v>
+                  <c:v>1.972592498039738</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>49.850927259796812</c:v>
+                  <c:v>0.14907274020318795</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>51.674447017633362</c:v>
+                  <c:v>-1.6744470176333621</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>53.497966775469976</c:v>
+                  <c:v>-3.4979667754699726</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>55.321486533306526</c:v>
+                  <c:v>-5.3214865333065227</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>57.145006291143133</c:v>
+                  <c:v>-7.1450062911431331</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>58.968526048979683</c:v>
+                  <c:v>-8.9685260489796832</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>60.792045806816233</c:v>
+                  <c:v>-10.792045806816233</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>62.615565564652847</c:v>
+                  <c:v>-12.615565564652847</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>64.439085322489404</c:v>
+                  <c:v>-14.439085322489397</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>66.262605080326011</c:v>
+                  <c:v>-16.262605080326011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4165,112 +4165,112 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>50</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>52</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>54</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>56</c:v>
+                  <c:v>-6</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>58</c:v>
+                  <c:v>-8</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>60</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>62</c:v>
+                  <c:v>-12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>64</c:v>
+                  <c:v>-14</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>66</c:v>
+                  <c:v>-16</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>68</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>70</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8046,16 +8046,16 @@
         <v>205</v>
       </c>
       <c r="B2" s="1">
-        <f>IF((3.3*A2/1023)&gt;0.7012,25-(0.7012-(3.3*A2/1023))/0.001769,25-(0.7012-(3.3*A2/1023))/0.001646)</f>
-        <v>0.75353741229956483</v>
+        <f>IF((3.3*A2/1023)&gt;0.7012,25-((3.3*A2/1023)-0.7012)/0.001769,25-((3.3*A2/1023)-0.7012)/0.001646)</f>
+        <v>49.246462587700435</v>
       </c>
       <c r="C2" s="4">
-        <f>2*A2 -410</f>
-        <v>0</v>
+        <f>(230-A2)*2</f>
+        <v>50</v>
       </c>
       <c r="D2" s="4">
         <f>ROUND(B2-C2, 0)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -8063,16 +8063,16 @@
         <v>206</v>
       </c>
       <c r="B3" s="1">
-        <f t="shared" ref="B3:B37" si="0">IF((3.3*A3/1023)&gt;0.7012,25-(0.7012-(3.3*A3/1023))/0.001769,25-(0.7012-(3.3*A3/1023))/0.001646)</f>
-        <v>2.7133226198407883</v>
+        <f t="shared" ref="B3:B37" si="0">IF((3.3*A3/1023)&gt;0.7012,25-((3.3*A3/1023)-0.7012)/0.001769,25-((3.3*A3/1023)-0.7012)/0.001646)</f>
+        <v>47.286677380159212</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C37" si="1">2*A3 -410</f>
-        <v>2</v>
+        <f t="shared" ref="C3:C37" si="1">(230-A3)*2</f>
+        <v>48</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D37" si="2">ROUND(B3-C3, 0)</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -8081,15 +8081,15 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
-        <v>4.6731078273820117</v>
+        <v>45.326892172617988</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -8098,15 +8098,15 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>6.6328930349233062</v>
+        <v>43.367106965076694</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -8115,15 +8115,15 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>8.5926782424645296</v>
+        <v>41.40732175753547</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -8132,15 +8132,15 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>10.552463450005822</v>
+        <v>39.447536549994176</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -8149,15 +8149,15 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>12.512248657547048</v>
+        <v>37.487751342452952</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -8166,11 +8166,11 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>14.472033865088273</v>
+        <v>35.527966134911729</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="2"/>
@@ -8183,11 +8183,11 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>16.431819072629565</v>
+        <v>33.568180927370435</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="2"/>
@@ -8200,11 +8200,11 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>18.391604280170856</v>
+        <v>31.608395719829144</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="2"/>
@@ -8217,11 +8217,11 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>20.351389487712147</v>
+        <v>29.648610512287853</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="2"/>
@@ -8234,11 +8234,11 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>22.311174695253374</v>
+        <v>27.688825304746626</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D13" s="4">
         <f t="shared" si="2"/>
@@ -8251,11 +8251,11 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>24.270959902794598</v>
+        <v>25.729040097205402</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4">
         <f t="shared" si="2"/>
@@ -8268,11 +8268,11 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>26.145170407921356</v>
+        <v>23.854829592078644</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="4">
         <f t="shared" si="2"/>
@@ -8285,11 +8285,11 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>27.968690165757906</v>
+        <v>22.031309834242094</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4">
         <f t="shared" si="2"/>
@@ -8302,11 +8302,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>29.792209923594516</v>
+        <v>20.207790076405484</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D17" s="4">
         <f t="shared" si="2"/>
@@ -8319,11 +8319,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" si="0"/>
-        <v>31.615729681431066</v>
+        <v>18.384270318568934</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D18" s="4">
         <f t="shared" si="2"/>
@@ -8336,15 +8336,15 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>33.439249439267613</v>
+        <v>16.560750560732384</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D19" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -8353,15 +8353,15 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" si="0"/>
-        <v>35.262769197104227</v>
+        <v>14.737230802895771</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D20" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -8370,15 +8370,15 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" si="0"/>
-        <v>37.086288954940777</v>
+        <v>12.913711045059223</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -8387,15 +8387,15 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" si="0"/>
-        <v>38.909808712777391</v>
+        <v>11.090191287222611</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D22" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -8404,15 +8404,15 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" si="0"/>
-        <v>40.733328470613941</v>
+        <v>9.2666715293860609</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D23" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -8421,15 +8421,15 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" si="0"/>
-        <v>42.556848228450491</v>
+        <v>7.4431517715495126</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="D24" s="4">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -8438,15 +8438,15 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" si="0"/>
-        <v>44.380367986287098</v>
+        <v>5.6196320137128986</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -8455,15 +8455,15 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" si="0"/>
-        <v>46.203887744123648</v>
+        <v>3.7961122558763485</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -8472,15 +8472,15 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" si="0"/>
-        <v>48.027407501960262</v>
+        <v>1.972592498039738</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -8489,15 +8489,15 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" si="0"/>
-        <v>49.850927259796812</v>
+        <v>0.14907274020318795</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>-2</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -8506,15 +8506,15 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" si="0"/>
-        <v>51.674447017633362</v>
+        <v>-1.6744470176333621</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>-4</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -8523,15 +8523,15 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" si="0"/>
-        <v>53.497966775469976</v>
+        <v>-3.4979667754699726</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>-6</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -8540,15 +8540,15 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" si="0"/>
-        <v>55.321486533306526</v>
+        <v>-5.3214865333065227</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>-8</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -8557,15 +8557,15 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" si="0"/>
-        <v>57.145006291143133</v>
+        <v>-7.1450062911431331</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>-10</v>
       </c>
       <c r="D32" s="4">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -8574,15 +8574,15 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" si="0"/>
-        <v>58.968526048979683</v>
+        <v>-8.9685260489796832</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>-12</v>
       </c>
       <c r="D33" s="4">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -8591,15 +8591,15 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" si="0"/>
-        <v>60.792045806816233</v>
+        <v>-10.792045806816233</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>-14</v>
       </c>
       <c r="D34" s="4">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -8608,15 +8608,15 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" si="0"/>
-        <v>62.615565564652847</v>
+        <v>-12.615565564652847</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>-16</v>
       </c>
       <c r="D35" s="4">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -8625,15 +8625,15 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" si="0"/>
-        <v>64.439085322489404</v>
+        <v>-14.439085322489397</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>-18</v>
       </c>
       <c r="D36" s="4">
         <f t="shared" si="2"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -8642,15 +8642,15 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" si="0"/>
-        <v>66.262605080326011</v>
+        <v>-16.262605080326011</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>-20</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="2"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>